<commit_message>
added m1,2,3 and changes in row S,R
</commit_message>
<xml_diff>
--- a/Master datasheet.xlsx
+++ b/Master datasheet.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20416"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\datacompilation\DataCompilation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A4234F-EAD6-4EA9-902E-1652371FD871}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="23040" windowHeight="9000" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="MASTER" sheetId="1" r:id="rId1"/>
@@ -22,11 +16,24 @@
     <sheet name="Sheet1" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="131">
   <si>
     <t>Company</t>
   </si>
@@ -166,24 +173,24 @@
     <t>P</t>
   </si>
   <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
     <t>N</t>
   </si>
   <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>U</t>
-  </si>
-  <si>
     <t>Z</t>
   </si>
   <si>
@@ -233,6 +240,15 @@
   </si>
   <si>
     <t>BA</t>
+  </si>
+  <si>
+    <t>BD</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>BF</t>
   </si>
   <si>
     <t>Company name</t>
@@ -415,8 +431,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -432,8 +454,152 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -442,36 +608,222 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79995117038483843"/>
+        <fgColor theme="7" tint="0.799951170384838"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79995117038483843"/>
+        <fgColor theme="5" tint="0.799951170384838"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79995117038483843"/>
+        <fgColor theme="4" tint="0.799951170384838"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79995117038483843"/>
+        <fgColor theme="6" tint="0.799951170384838"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79995117038483843"/>
+        <fgColor theme="9" tint="0.799951170384838"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -494,9 +846,251 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -507,6 +1101,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -516,24 +1116,62 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -791,132 +1429,134 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:AB1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="A1" sqref="$A1:$XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="19.2" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="19.2" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="4" customWidth="1"/>
-    <col min="2" max="9" width="8.88671875" style="5"/>
-    <col min="10" max="15" width="8.88671875" style="6"/>
-    <col min="16" max="20" width="8.88671875" style="7"/>
-    <col min="21" max="24" width="8.88671875" style="8"/>
-    <col min="25" max="27" width="8.88671875" style="9"/>
-    <col min="28" max="16384" width="8.88671875" style="4"/>
+    <col min="1" max="1" width="8.88888888888889" style="6" customWidth="1"/>
+    <col min="2" max="9" width="8.88888888888889" style="7"/>
+    <col min="10" max="15" width="8.88888888888889" style="8"/>
+    <col min="16" max="20" width="8.88888888888889" style="9"/>
+    <col min="21" max="24" width="8.88888888888889" style="10"/>
+    <col min="25" max="27" width="8.88888888888889" style="11"/>
+    <col min="28" max="16384" width="8.88888888888889" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="19.2" customHeight="1">
-      <c r="A1" s="4" t="s">
+    <row r="1" customHeight="1" spans="1:28">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="R1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="S1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="T1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="U1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="V1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="W1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="X1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="10" t="s">
+      <c r="Y1" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="10" t="s">
+      <c r="Z1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="10" t="s">
+      <c r="AA1" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AB1" s="6" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+      <selection activeCell="A14" sqref="$A14:$XFD14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" customWidth="1"/>
+    <col min="1" max="1" width="8.88888888888889" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1025,10 +1665,10 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1041,7 +1681,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>42</v>
@@ -1049,7 +1689,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>44</v>
@@ -1057,15 +1697,15 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>40</v>
@@ -1076,7 +1716,7 @@
         <v>31</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1084,7 +1724,7 @@
         <v>33</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1121,21 +1761,23 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection activeCell="A10" sqref="$A10:$XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="7"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -1257,7 +1899,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>36</v>
@@ -1299,7 +1941,7 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>39</v>
@@ -1313,7 +1955,7 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>53</v>
@@ -1327,7 +1969,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>52</v>
@@ -1344,7 +1986,7 @@
         <v>55</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -1358,7 +2000,7 @@
         <v>58</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -1529,21 +2171,23 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="A9" sqref="$A9:$XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="7"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -1552,18 +2196,18 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
@@ -1665,7 +2309,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>45</v>
@@ -1707,7 +2351,7 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>38</v>
@@ -1721,7 +2365,7 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>39</v>
@@ -1735,7 +2379,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>40</v>
@@ -1752,7 +2396,7 @@
         <v>31</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -1766,7 +2410,7 @@
         <v>33</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -1833,21 +2477,23 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:H21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="7"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -1856,18 +2502,18 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
@@ -2042,7 +2688,7 @@
         <v>65</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -2051,12 +2697,12 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1">
+    <row r="16" ht="15" customHeight="1" spans="1:8">
       <c r="A16" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -2122,8 +2768,12 @@
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
+      <c r="A21" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -2131,22 +2781,40 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="A9" sqref="$A9:$XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="7"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -2155,18 +2823,18 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
@@ -2282,7 +2950,7 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>38</v>
@@ -2296,7 +2964,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>39</v>
@@ -2310,10 +2978,10 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -2338,7 +3006,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>40</v>
@@ -2355,7 +3023,7 @@
         <v>31</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -2369,7 +3037,7 @@
         <v>33</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -2422,12 +3090,14 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:J58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2437,12 +3107,12 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
+      <c r="A1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -2452,41 +3122,41 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1"/>
-      <c r="B2" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
+      <c r="B2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1"/>
-      <c r="B3" s="3" t="s">
-        <v>71</v>
+      <c r="B3" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
+        <v>75</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -2499,10 +3169,10 @@
     <row r="5" spans="1:10">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -2515,10 +3185,10 @@
     <row r="6" spans="1:10">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -2531,10 +3201,10 @@
     <row r="7" spans="1:10">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -2547,10 +3217,10 @@
     <row r="8" spans="1:10">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -2563,10 +3233,10 @@
     <row r="9" spans="1:10">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -2579,10 +3249,10 @@
     <row r="10" spans="1:10">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -2595,10 +3265,10 @@
     <row r="11" spans="1:10">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -2611,10 +3281,10 @@
     <row r="12" spans="1:10">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -2627,10 +3297,10 @@
     <row r="13" spans="1:10">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -2643,10 +3313,10 @@
     <row r="14" spans="1:10">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -2659,10 +3329,10 @@
     <row r="15" spans="1:10">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -2675,10 +3345,10 @@
     <row r="16" spans="1:10">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -2691,10 +3361,10 @@
     <row r="17" spans="1:10">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -2707,10 +3377,10 @@
     <row r="18" spans="1:10">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -2723,10 +3393,10 @@
     <row r="19" spans="1:10">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -2739,10 +3409,10 @@
     <row r="20" spans="1:10">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -2755,10 +3425,10 @@
     <row r="21" spans="1:10">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -2771,10 +3441,10 @@
     <row r="22" spans="1:10">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -2787,10 +3457,10 @@
     <row r="23" spans="1:10">
       <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -2803,10 +3473,10 @@
     <row r="24" spans="1:10">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -2819,10 +3489,10 @@
     <row r="25" spans="1:10">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -2835,10 +3505,10 @@
     <row r="26" spans="1:10">
       <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -2851,10 +3521,10 @@
     <row r="27" spans="1:10">
       <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -2867,10 +3537,10 @@
     <row r="28" spans="1:10">
       <c r="A28" s="2"/>
       <c r="B28" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -2883,10 +3553,10 @@
     <row r="29" spans="1:10">
       <c r="A29" s="2"/>
       <c r="B29" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -2899,10 +3569,10 @@
     <row r="30" spans="1:10">
       <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -2915,10 +3585,10 @@
     <row r="31" spans="1:10">
       <c r="A31" s="2"/>
       <c r="B31" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -2931,10 +3601,10 @@
     <row r="32" spans="1:10">
       <c r="A32" s="2"/>
       <c r="B32" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -2947,10 +3617,10 @@
     <row r="33" spans="1:10">
       <c r="A33" s="2"/>
       <c r="B33" s="2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -2963,10 +3633,10 @@
     <row r="34" spans="1:10">
       <c r="A34" s="2"/>
       <c r="B34" s="2" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -2979,10 +3649,10 @@
     <row r="35" spans="1:10">
       <c r="A35" s="2"/>
       <c r="B35" s="2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -2995,10 +3665,10 @@
     <row r="36" spans="1:10">
       <c r="A36" s="2"/>
       <c r="B36" s="2" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -3011,10 +3681,10 @@
     <row r="37" spans="1:10">
       <c r="A37" s="2"/>
       <c r="B37" s="2" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -3027,10 +3697,10 @@
     <row r="38" spans="1:10">
       <c r="A38" s="2"/>
       <c r="B38" s="2" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -3043,10 +3713,10 @@
     <row r="39" spans="1:10">
       <c r="A39" s="2"/>
       <c r="B39" s="2" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -3059,10 +3729,10 @@
     <row r="40" spans="1:10">
       <c r="A40" s="2"/>
       <c r="B40" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -3075,10 +3745,10 @@
     <row r="41" spans="1:10">
       <c r="A41" s="2"/>
       <c r="B41" s="2" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -3091,10 +3761,10 @@
     <row r="42" spans="1:10">
       <c r="A42" s="2"/>
       <c r="B42" s="2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -3107,10 +3777,10 @@
     <row r="43" spans="1:10">
       <c r="A43" s="2"/>
       <c r="B43" s="2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -3123,10 +3793,10 @@
     <row r="44" spans="1:10">
       <c r="A44" s="2"/>
       <c r="B44" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -3139,10 +3809,10 @@
     <row r="45" spans="1:10">
       <c r="A45" s="2"/>
       <c r="B45" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -3155,10 +3825,10 @@
     <row r="46" spans="1:10">
       <c r="A46" s="2"/>
       <c r="B46" s="2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -3171,10 +3841,10 @@
     <row r="47" spans="1:10">
       <c r="A47" s="2"/>
       <c r="B47" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -3187,10 +3857,10 @@
     <row r="48" spans="1:10">
       <c r="A48" s="2"/>
       <c r="B48" s="2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -3203,10 +3873,10 @@
     <row r="49" spans="1:10">
       <c r="A49" s="2"/>
       <c r="B49" s="2" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
@@ -3219,10 +3889,10 @@
     <row r="50" spans="1:10">
       <c r="A50" s="2"/>
       <c r="B50" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
@@ -3235,10 +3905,10 @@
     <row r="51" spans="1:10">
       <c r="A51" s="2"/>
       <c r="B51" s="2" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -3251,10 +3921,10 @@
     <row r="52" spans="1:10">
       <c r="A52" s="2"/>
       <c r="B52" s="2" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
@@ -3267,10 +3937,10 @@
     <row r="53" spans="1:10">
       <c r="A53" s="2"/>
       <c r="B53" s="2" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
@@ -3283,10 +3953,10 @@
     <row r="54" spans="1:10">
       <c r="A54" s="2"/>
       <c r="B54" s="2" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
@@ -3299,10 +3969,10 @@
     <row r="55" spans="1:10">
       <c r="A55" s="2"/>
       <c r="B55" s="2" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -3315,10 +3985,10 @@
     <row r="56" spans="1:10">
       <c r="A56" s="2"/>
       <c r="B56" s="2" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
@@ -3331,10 +4001,10 @@
     <row r="57" spans="1:10">
       <c r="A57" s="2"/>
       <c r="B57" s="2" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
@@ -3347,10 +4017,10 @@
     <row r="58" spans="1:10">
       <c r="A58" s="2"/>
       <c r="B58" s="2" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
@@ -3366,6 +4036,7 @@
     <mergeCell ref="B2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
little changes from naman
</commit_message>
<xml_diff>
--- a/Master datasheet.xlsx
+++ b/Master datasheet.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20416"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\datacompilation\DataCompilation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD3D84E-2C49-46A7-9F83-A0F101C90FA1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MASTER" sheetId="1" r:id="rId1"/>
@@ -16,24 +22,11 @@
     <sheet name="Sheet1" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="135">
   <si>
     <t>Company</t>
   </si>
@@ -443,14 +436,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="21">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -466,152 +453,8 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="38">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -620,222 +463,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799951170384838"/>
+        <fgColor theme="7" tint="0.79992065187536243"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799951170384838"/>
+        <fgColor theme="5" tint="0.79992065187536243"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799951170384838"/>
+        <fgColor theme="4" tint="0.79992065187536243"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799951170384838"/>
+        <fgColor theme="6" tint="0.79992065187536243"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799951170384838"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.79992065187536243"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -858,262 +515,17 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1125,62 +537,24 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Percent" xfId="3" builtinId="5"/>
-    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
-    <cellStyle name="Note" xfId="8" builtinId="10"/>
-    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
-    <cellStyle name="Title" xfId="10" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
-    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
-    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
-    <cellStyle name="Input" xfId="16" builtinId="20"/>
-    <cellStyle name="Output" xfId="17" builtinId="21"/>
-    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
-    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
-    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
-    <cellStyle name="Total" xfId="21" builtinId="25"/>
-    <cellStyle name="Good" xfId="22" builtinId="26"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1438,134 +812,132 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="19.2" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="19.2" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.88888888888889" style="5" customWidth="1"/>
-    <col min="2" max="9" width="8.88888888888889" style="6"/>
-    <col min="10" max="15" width="8.88888888888889" style="7"/>
-    <col min="16" max="20" width="8.88888888888889" style="8"/>
-    <col min="21" max="24" width="8.88888888888889" style="9"/>
-    <col min="25" max="27" width="8.88888888888889" style="10"/>
-    <col min="28" max="16384" width="8.88888888888889" style="5"/>
+    <col min="1" max="1" width="8.88671875" style="4" customWidth="1"/>
+    <col min="2" max="9" width="8.88671875" style="5"/>
+    <col min="10" max="15" width="8.88671875" style="6"/>
+    <col min="16" max="20" width="8.88671875" style="7"/>
+    <col min="21" max="24" width="8.88671875" style="8"/>
+    <col min="25" max="27" width="8.88671875" style="9"/>
+    <col min="28" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:28">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:28" ht="19.2" customHeight="1">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="P1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Q1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="S1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="T1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="9" t="s">
+      <c r="U1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="9" t="s">
+      <c r="V1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="9" t="s">
+      <c r="W1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="9" t="s">
+      <c r="X1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="11" t="s">
+      <c r="Y1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="11" t="s">
+      <c r="Z1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="11" t="s">
+      <c r="AA1" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AB1" s="4" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.88888888888889" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1596,7 +968,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>35</v>
       </c>
@@ -1604,7 +976,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>37</v>
       </c>
@@ -1612,7 +984,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>38</v>
       </c>
@@ -1620,7 +992,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
         <v>39</v>
       </c>
@@ -1628,7 +1000,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
         <v>40</v>
       </c>
@@ -1636,7 +1008,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
         <v>41</v>
       </c>
@@ -1644,7 +1016,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
         <v>42</v>
       </c>
@@ -1652,7 +1024,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
         <v>43</v>
       </c>
@@ -1660,7 +1032,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
         <v>44</v>
       </c>
@@ -1668,7 +1040,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
         <v>45</v>
       </c>
@@ -1676,7 +1048,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
         <v>47</v>
       </c>
@@ -1684,7 +1056,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
         <v>49</v>
       </c>
@@ -1692,7 +1064,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
         <v>46</v>
       </c>
@@ -1700,7 +1072,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
         <v>51</v>
       </c>
@@ -1774,23 +1146,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -2180,43 +1550,51 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="$A9:$XFD9"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>28</v>
       </c>
       <c r="B1" t="s">
         <v>29</v>
       </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="C2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
@@ -2486,23 +1864,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -2517,22 +1893,22 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
@@ -2716,7 +2092,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" ht="15" customHeight="1" spans="1:8">
+    <row r="16" spans="1:8" ht="15" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>67</v>
       </c>
@@ -2786,7 +2162,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:8">
       <c r="A21" s="2" t="s">
         <v>72</v>
       </c>
@@ -2794,7 +2170,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:8">
       <c r="A22" s="2" t="s">
         <v>73</v>
       </c>
@@ -2804,25 +2180,23 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="2" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>28</v>
       </c>
@@ -2837,10 +2211,10 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -2849,10 +2223,10 @@
       <c r="D2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
@@ -3092,7 +2466,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:8">
       <c r="A20" s="2" t="s">
         <v>70</v>
       </c>
@@ -3100,7 +2474,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:8">
       <c r="A21" s="2" t="s">
         <v>74</v>
       </c>
@@ -3108,7 +2482,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:8">
       <c r="A22" s="2" t="s">
         <v>75</v>
       </c>
@@ -3118,29 +2492,27 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -3150,33 +2522,33 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1"/>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1"/>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>78</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="2"/>
@@ -4064,7 +3436,6 @@
     <mergeCell ref="B2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added multiple file and database connectivity
</commit_message>
<xml_diff>
--- a/Master datasheet.xlsx
+++ b/Master datasheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000" activeTab="6"/>
+    <workbookView windowWidth="23040" windowHeight="9000" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="MASTER" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="85">
   <si>
     <t>Company</t>
   </si>
@@ -238,6 +238,15 @@
     <t>AN</t>
   </si>
   <si>
+    <t>BD</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>BF</t>
+  </si>
+  <si>
     <t>AJ</t>
   </si>
   <si>
@@ -250,27 +259,12 @@
     <t>BA</t>
   </si>
   <si>
-    <t>BD</t>
-  </si>
-  <si>
-    <t>BE</t>
-  </si>
-  <si>
-    <t>BF</t>
-  </si>
-  <si>
     <t>BB</t>
   </si>
   <si>
     <t>BC</t>
   </si>
   <si>
-    <t xml:space="preserve">To </t>
-  </si>
-  <si>
-    <t>StfRf</t>
-  </si>
-  <si>
     <t>AK</t>
   </si>
   <si>
@@ -284,6 +278,18 @@
   </si>
   <si>
     <t>CC</t>
+  </si>
+  <si>
+    <t>CG</t>
+  </si>
+  <si>
+    <t>CH</t>
+  </si>
+  <si>
+    <t>CI</t>
+  </si>
+  <si>
+    <t>AH</t>
   </si>
 </sst>
 </file>
@@ -1278,8 +1284,8 @@
   <sheetPr/>
   <dimension ref="A1:AB1"/>
   <sheetViews>
-    <sheetView zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1"/>
+    <sheetView zoomScale="81" zoomScaleNormal="81" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q$1:Q$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="19.2" customHeight="1"/>
@@ -1617,7 +1623,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="7"/>
@@ -2020,10 +2026,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="7"/>
@@ -2043,11 +2049,11 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>65</v>
+      <c r="A2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>35</v>
@@ -2062,10 +2068,10 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -2076,10 +2082,10 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -2090,10 +2096,10 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -2104,10 +2110,10 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -2118,10 +2124,10 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -2132,10 +2138,10 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -2146,10 +2152,10 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -2160,10 +2166,10 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -2174,10 +2180,10 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -2188,10 +2194,10 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -2202,10 +2208,10 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -2216,10 +2222,10 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -2230,10 +2236,10 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -2244,10 +2250,10 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -2258,10 +2264,10 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -2272,10 +2278,10 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -2286,10 +2292,10 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -2300,10 +2306,10 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -2314,10 +2320,10 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -2325,6 +2331,22 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2560,7 +2582,7 @@
     </row>
     <row r="16" ht="15" customHeight="1" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>49</v>
@@ -2574,7 +2596,7 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>57</v>
@@ -2588,7 +2610,7 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>58</v>
@@ -2602,7 +2624,7 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>48</v>
@@ -2616,7 +2638,7 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>44</v>
@@ -2630,7 +2652,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>45</v>
@@ -2638,7 +2660,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>47</v>
@@ -2656,7 +2678,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="7"/>
@@ -2922,7 +2944,7 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>57</v>
@@ -2936,7 +2958,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>44</v>
@@ -2968,10 +2990,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -2981,13 +3003,13 @@
         <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" t="s">
-        <v>77</v>
+      <c r="D1" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3130,6 +3152,30 @@
       </c>
       <c r="B18" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -3141,10 +3187,10 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -3275,7 +3321,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B15" t="s">
         <v>43</v>
@@ -3283,7 +3329,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B16" t="s">
         <v>55</v>
@@ -3299,7 +3345,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B18" t="s">
         <v>53</v>
@@ -3307,7 +3353,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B19" t="s">
         <v>57</v>
@@ -3315,10 +3361,34 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B20" t="s">
         <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -3330,10 +3400,10 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -3348,8 +3418,8 @@
       <c r="C1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" t="s">
-        <v>77</v>
+      <c r="D1" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3492,6 +3562,30 @@
       </c>
       <c r="B18" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>